<commit_message>
for 30 cases working fine
</commit_message>
<xml_diff>
--- a/Code/Results/Cases/Case_000/res_bus/vm_pu.xlsx
+++ b/Code/Results/Cases/Case_000/res_bus/vm_pu.xlsx
@@ -433,16 +433,16 @@
         <v>1.05</v>
       </c>
       <c r="C2">
-        <v>0.9980342968504127</v>
+        <v>0.9980342968504132</v>
       </c>
       <c r="D2">
-        <v>1.020227969265645</v>
+        <v>1.020227969265646</v>
       </c>
       <c r="E2">
-        <v>1.00234269268442</v>
+        <v>1.002342692684421</v>
       </c>
       <c r="F2">
-        <v>1.015770724134319</v>
+        <v>1.01577072413432</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -451,7 +451,7 @@
         <v>1.046782275101134</v>
       </c>
       <c r="J2">
-        <v>1.020273961143927</v>
+        <v>1.020273961143928</v>
       </c>
       <c r="K2">
         <v>1.031412509617071</v>
@@ -460,16 +460,16 @@
         <v>1.013769486278824</v>
       </c>
       <c r="M2">
-        <v>1.027014634443499</v>
+        <v>1.0270146344435</v>
       </c>
       <c r="N2">
-        <v>1.02172286719581</v>
+        <v>1.021722867195811</v>
       </c>
       <c r="O2">
         <v>1.03</v>
       </c>
       <c r="P2">
-        <v>1.029952583034311</v>
+        <v>1.029952583034312</v>
       </c>
       <c r="Q2">
         <v>1.02</v>
@@ -486,13 +486,13 @@
         <v>1.05</v>
       </c>
       <c r="C3">
-        <v>1.004825848129952</v>
+        <v>1.004825848129953</v>
       </c>
       <c r="D3">
-        <v>1.024987077111014</v>
+        <v>1.024987077111015</v>
       </c>
       <c r="E3">
-        <v>1.008245117487965</v>
+        <v>1.008245117487966</v>
       </c>
       <c r="F3">
         <v>1.020117966595953</v>
@@ -504,19 +504,19 @@
         <v>1.04870362624981</v>
       </c>
       <c r="J3">
-        <v>1.025185814633747</v>
+        <v>1.025185814633748</v>
       </c>
       <c r="K3">
-        <v>1.035309922471374</v>
+        <v>1.035309922471375</v>
       </c>
       <c r="L3">
-        <v>1.018773576396161</v>
+        <v>1.018773576396162</v>
       </c>
       <c r="M3">
-        <v>1.030499746114025</v>
+        <v>1.030499746114026</v>
       </c>
       <c r="N3">
-        <v>1.026641696080983</v>
+        <v>1.026641696080985</v>
       </c>
       <c r="O3">
         <v>1.03</v>
@@ -539,13 +539,13 @@
         <v>1.05</v>
       </c>
       <c r="C4">
-        <v>1.009085692487844</v>
+        <v>1.009085692487845</v>
       </c>
       <c r="D4">
-        <v>1.027974097629449</v>
+        <v>1.02797409762945</v>
       </c>
       <c r="E4">
-        <v>1.011947723393484</v>
+        <v>1.011947723393485</v>
       </c>
       <c r="F4">
         <v>1.0228611408862</v>
@@ -554,28 +554,28 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <v>1.049892112496764</v>
+        <v>1.049892112496765</v>
       </c>
       <c r="J4">
         <v>1.028259806579122</v>
       </c>
       <c r="K4">
-        <v>1.037746227913402</v>
+        <v>1.037746227913403</v>
       </c>
       <c r="L4">
-        <v>1.021904057246477</v>
+        <v>1.021904057246478</v>
       </c>
       <c r="M4">
         <v>1.032691264740112</v>
       </c>
       <c r="N4">
-        <v>1.029720053447512</v>
+        <v>1.029720053447513</v>
       </c>
       <c r="O4">
         <v>1.03</v>
       </c>
       <c r="P4">
-        <v>1.034445307860265</v>
+        <v>1.034445307860266</v>
       </c>
       <c r="Q4">
         <v>1.02</v>
@@ -592,16 +592,16 @@
         <v>1.05</v>
       </c>
       <c r="C5">
-        <v>1.010860465115728</v>
+        <v>1.010860465115729</v>
       </c>
       <c r="D5">
-        <v>1.02922095230947</v>
+        <v>1.029220952309471</v>
       </c>
       <c r="E5">
         <v>1.013496114626757</v>
       </c>
       <c r="F5">
-        <v>1.024004762544206</v>
+        <v>1.024004762544205</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -628,7 +628,7 @@
         <v>1.03</v>
       </c>
       <c r="P5">
-        <v>1.035167914055625</v>
+        <v>1.035167914055624</v>
       </c>
       <c r="Q5">
         <v>1.02</v>
@@ -672,7 +672,7 @@
         <v>1.023454325624266</v>
       </c>
       <c r="M6">
-        <v>1.033764303679491</v>
+        <v>1.03376430367949</v>
       </c>
       <c r="N6">
         <v>1.031236133386631</v>
@@ -681,7 +681,7 @@
         <v>1.03</v>
       </c>
       <c r="P6">
-        <v>1.035294552937739</v>
+        <v>1.035294552937738</v>
       </c>
       <c r="Q6">
         <v>1.02</v>
@@ -698,13 +698,13 @@
         <v>1.05</v>
       </c>
       <c r="C7">
-        <v>1.009157878763058</v>
+        <v>1.009157878763059</v>
       </c>
       <c r="D7">
-        <v>1.028031265494132</v>
+        <v>1.028031265494133</v>
       </c>
       <c r="E7">
-        <v>1.012029831323298</v>
+        <v>1.012029831323299</v>
       </c>
       <c r="F7">
         <v>1.02289738356868</v>
@@ -716,13 +716,13 @@
         <v>1.049919311533003</v>
       </c>
       <c r="J7">
-        <v>1.028324184982367</v>
+        <v>1.028324184982368</v>
       </c>
       <c r="K7">
-        <v>1.037799859398269</v>
+        <v>1.03779985939827</v>
       </c>
       <c r="L7">
-        <v>1.021982249600055</v>
+        <v>1.021982249600057</v>
       </c>
       <c r="M7">
         <v>1.032724182413771</v>
@@ -740,7 +740,7 @@
         <v>1.02</v>
       </c>
       <c r="R7">
-        <v>1.03781642257104</v>
+        <v>1.037816422571041</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -751,13 +751,13 @@
         <v>1.05</v>
       </c>
       <c r="C8">
-        <v>1.000422998057982</v>
+        <v>1.000422998057984</v>
       </c>
       <c r="D8">
-        <v>1.02190923803408</v>
+        <v>1.021909238034081</v>
       </c>
       <c r="E8">
-        <v>1.004444794149335</v>
+        <v>1.004444794149336</v>
       </c>
       <c r="F8">
         <v>1.017282794957548</v>
@@ -766,34 +766,34 @@
         <v>1</v>
       </c>
       <c r="I8">
-        <v>1.047470227810798</v>
+        <v>1.047470227810799</v>
       </c>
       <c r="J8">
-        <v>1.022018937152989</v>
+        <v>1.02201893715299</v>
       </c>
       <c r="K8">
-        <v>1.032800392690884</v>
+        <v>1.032800392690885</v>
       </c>
       <c r="L8">
-        <v>1.015564892615661</v>
+        <v>1.015564892615663</v>
       </c>
       <c r="M8">
         <v>1.028233640150378</v>
       </c>
       <c r="N8">
-        <v>1.023470321270956</v>
+        <v>1.023470321270958</v>
       </c>
       <c r="O8">
         <v>1.03</v>
       </c>
       <c r="P8">
-        <v>1.030917358042472</v>
+        <v>1.030917358042473</v>
       </c>
       <c r="Q8">
         <v>1.02</v>
       </c>
       <c r="R8">
-        <v>1.034285978964663</v>
+        <v>1.034285978964664</v>
       </c>
     </row>
     <row r="9" spans="1:18">
@@ -804,16 +804,16 @@
         <v>1.05</v>
       </c>
       <c r="C9">
-        <v>0.9838299771539669</v>
+        <v>0.9838299771539655</v>
       </c>
       <c r="D9">
-        <v>1.010291247722008</v>
+        <v>1.010291247722007</v>
       </c>
       <c r="E9">
-        <v>0.9900072044196317</v>
+        <v>0.9900072044196302</v>
       </c>
       <c r="F9">
-        <v>1.006776813612214</v>
+        <v>1.006776813612212</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -822,31 +822,31 @@
         <v>1.042674631510305</v>
       </c>
       <c r="J9">
-        <v>1.009966952910883</v>
+        <v>1.009966952910881</v>
       </c>
       <c r="K9">
-        <v>1.02321953441111</v>
+        <v>1.023219534411108</v>
       </c>
       <c r="L9">
-        <v>1.003264515415473</v>
+        <v>1.003264515415472</v>
       </c>
       <c r="M9">
-        <v>1.019760890331668</v>
+        <v>1.019760890331666</v>
       </c>
       <c r="N9">
-        <v>1.011401221828846</v>
+        <v>1.011401221828844</v>
       </c>
       <c r="O9">
         <v>1.03</v>
       </c>
       <c r="P9">
-        <v>1.024211621336737</v>
+        <v>1.024211621336735</v>
       </c>
       <c r="Q9">
         <v>1.02</v>
       </c>
       <c r="R9">
-        <v>1.02750830962907</v>
+        <v>1.027508309629069</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -857,16 +857,16 @@
         <v>1.05</v>
       </c>
       <c r="C10">
-        <v>0.9723181722952661</v>
+        <v>0.972318172295267</v>
       </c>
       <c r="D10">
-        <v>1.002263909463432</v>
+        <v>1.002263909463433</v>
       </c>
       <c r="E10">
-        <v>0.9801160008376614</v>
+        <v>0.9801160008376619</v>
       </c>
       <c r="F10">
-        <v>0.9997968719731501</v>
+        <v>0.9997968719731504</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -875,19 +875,19 @@
         <v>1.039296535362348</v>
       </c>
       <c r="J10">
-        <v>1.001674821119869</v>
+        <v>1.00167482111987</v>
       </c>
       <c r="K10">
         <v>1.016592408280079</v>
       </c>
       <c r="L10">
-        <v>0.9948537937777644</v>
+        <v>0.9948537937777649</v>
       </c>
       <c r="M10">
-        <v>1.014169794928024</v>
+        <v>1.014169794928025</v>
       </c>
       <c r="N10">
-        <v>1.003097314259567</v>
+        <v>1.003097314259568</v>
       </c>
       <c r="O10">
         <v>1.03</v>
@@ -910,43 +910,43 @@
         <v>1.05</v>
       </c>
       <c r="C11">
-        <v>0.9705277986284097</v>
+        <v>0.9705277986284085</v>
       </c>
       <c r="D11">
-        <v>1.001092198471613</v>
+        <v>1.001092198471612</v>
       </c>
       <c r="E11">
-        <v>0.9795222450953974</v>
+        <v>0.9795222450953965</v>
       </c>
       <c r="F11">
-        <v>1.00038909227071</v>
+        <v>1.000389092270709</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="I11">
-        <v>1.038989145004962</v>
+        <v>1.038989145004961</v>
       </c>
       <c r="J11">
-        <v>1.001180217054234</v>
+        <v>1.001180217054233</v>
       </c>
       <c r="K11">
-        <v>1.015993546880684</v>
+        <v>1.015993546880683</v>
       </c>
       <c r="L11">
-        <v>0.9948409577526067</v>
+        <v>0.9948409577526057</v>
       </c>
       <c r="M11">
-        <v>1.015303674609896</v>
+        <v>1.015303674609895</v>
       </c>
       <c r="N11">
-        <v>1.002602007799427</v>
+        <v>1.002602007799426</v>
       </c>
       <c r="O11">
         <v>1.03</v>
       </c>
       <c r="P11">
-        <v>1.021181608748392</v>
+        <v>1.021181608748391</v>
       </c>
       <c r="Q11">
         <v>1.02</v>
@@ -963,16 +963,16 @@
         <v>1.05</v>
       </c>
       <c r="C12">
-        <v>0.9710029100469674</v>
+        <v>0.971002910046967</v>
       </c>
       <c r="D12">
         <v>1.001470170822472</v>
       </c>
       <c r="E12">
-        <v>0.9806197067019186</v>
+        <v>0.980619706701918</v>
       </c>
       <c r="F12">
-        <v>1.001846826566304</v>
+        <v>1.001846826566303</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -981,19 +981,19 @@
         <v>1.039284038361803</v>
       </c>
       <c r="J12">
-        <v>1.002087278051734</v>
+        <v>1.002087278051733</v>
       </c>
       <c r="K12">
         <v>1.016569258777887</v>
       </c>
       <c r="L12">
-        <v>0.9961278658058319</v>
+        <v>0.9961278658058315</v>
       </c>
       <c r="M12">
-        <v>1.016938729620794</v>
+        <v>1.016938729620793</v>
       </c>
       <c r="N12">
-        <v>1.003510356927585</v>
+        <v>1.003510356927584</v>
       </c>
       <c r="O12">
         <v>1.03</v>
@@ -1016,16 +1016,16 @@
         <v>1.05</v>
       </c>
       <c r="C13">
-        <v>0.9732950087471437</v>
+        <v>0.973295008747144</v>
       </c>
       <c r="D13">
         <v>1.003102440293322</v>
       </c>
       <c r="E13">
-        <v>0.9831452414563631</v>
+        <v>0.9831452414563635</v>
       </c>
       <c r="F13">
-        <v>1.004103644712398</v>
+        <v>1.004103644712397</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -1034,16 +1034,16 @@
         <v>1.040086511864439</v>
       </c>
       <c r="J13">
-        <v>1.004177273411231</v>
+        <v>1.004177273411232</v>
       </c>
       <c r="K13">
         <v>1.018126607812662</v>
       </c>
       <c r="L13">
-        <v>0.9985574896464287</v>
+        <v>0.9985574896464293</v>
       </c>
       <c r="M13">
-        <v>1.019108874184587</v>
+        <v>1.019108874184586</v>
       </c>
       <c r="N13">
         <v>1.005603320320219</v>
@@ -1052,7 +1052,7 @@
         <v>1.03</v>
       </c>
       <c r="P13">
-        <v>1.024803131659261</v>
+        <v>1.02480313165926</v>
       </c>
       <c r="Q13">
         <v>1.02</v>
@@ -1069,13 +1069,13 @@
         <v>1.05</v>
       </c>
       <c r="C14">
-        <v>0.9756700848390257</v>
+        <v>0.9756700848390266</v>
       </c>
       <c r="D14">
-        <v>1.004777848035159</v>
+        <v>1.00477784803516</v>
       </c>
       <c r="E14">
-        <v>0.9855059882995296</v>
+        <v>0.9855059882995306</v>
       </c>
       <c r="F14">
         <v>1.005998263165293</v>
@@ -1084,22 +1084,22 @@
         <v>1</v>
       </c>
       <c r="I14">
-        <v>1.040860224804681</v>
+        <v>1.040860224804682</v>
       </c>
       <c r="J14">
-        <v>1.00612840990464</v>
+        <v>1.006128409904641</v>
       </c>
       <c r="K14">
-        <v>1.019627071527975</v>
+        <v>1.019627071527976</v>
       </c>
       <c r="L14">
         <v>1.00072385186049</v>
       </c>
       <c r="M14">
-        <v>1.020824762322153</v>
+        <v>1.020824762322152</v>
       </c>
       <c r="N14">
-        <v>1.007557227651246</v>
+        <v>1.007557227651247</v>
       </c>
       <c r="O14">
         <v>1.03</v>
@@ -1111,7 +1111,7 @@
         <v>1.02</v>
       </c>
       <c r="R14">
-        <v>1.025017397503928</v>
+        <v>1.025017397503929</v>
       </c>
     </row>
     <row r="15" spans="1:18">
@@ -1122,7 +1122,7 @@
         <v>1.05</v>
       </c>
       <c r="C15">
-        <v>0.9766890399037615</v>
+        <v>0.9766890399037614</v>
       </c>
       <c r="D15">
         <v>1.005493490962952</v>
@@ -1152,7 +1152,7 @@
         <v>1.02142346443611</v>
       </c>
       <c r="N15">
-        <v>1.008337542971375</v>
+        <v>1.008337542971374</v>
       </c>
       <c r="O15">
         <v>1.03</v>
@@ -1175,13 +1175,13 @@
         <v>1.05</v>
       </c>
       <c r="C16">
-        <v>0.981023793764024</v>
+        <v>0.9810237937640245</v>
       </c>
       <c r="D16">
         <v>1.008510847687537</v>
       </c>
       <c r="E16">
-        <v>0.9900205441728952</v>
+        <v>0.9900205441728958</v>
       </c>
       <c r="F16">
         <v>1.009205213021962</v>
@@ -1199,10 +1199,10 @@
         <v>1.022691886422416</v>
       </c>
       <c r="L16">
-        <v>1.004535133840101</v>
+        <v>1.004535133840102</v>
       </c>
       <c r="M16">
-        <v>1.023374034552506</v>
+        <v>1.023374034552505</v>
       </c>
       <c r="N16">
         <v>1.01136602031819</v>
@@ -1211,7 +1211,7 @@
         <v>1.03</v>
       </c>
       <c r="P16">
-        <v>1.028348437766935</v>
+        <v>1.028348437766934</v>
       </c>
       <c r="Q16">
         <v>1.02</v>
@@ -1228,49 +1228,49 @@
         <v>1.05</v>
       </c>
       <c r="C17">
-        <v>0.9831433025220537</v>
+        <v>0.9831433025220521</v>
       </c>
       <c r="D17">
-        <v>1.009975796202422</v>
+        <v>1.009975796202421</v>
       </c>
       <c r="E17">
-        <v>0.9915735396652405</v>
+        <v>0.9915735396652389</v>
       </c>
       <c r="F17">
-        <v>1.010157380916862</v>
+        <v>1.01015738091686</v>
       </c>
       <c r="G17">
         <v>1</v>
       </c>
       <c r="I17">
-        <v>1.04300777484973</v>
+        <v>1.043007774849729</v>
       </c>
       <c r="J17">
-        <v>1.011265033981814</v>
+        <v>1.011265033981812</v>
       </c>
       <c r="K17">
-        <v>1.023811145572112</v>
+        <v>1.023811145572111</v>
       </c>
       <c r="L17">
-        <v>1.005730946195242</v>
+        <v>1.00573094619524</v>
       </c>
       <c r="M17">
-        <v>1.023989627906374</v>
+        <v>1.023989627906372</v>
       </c>
       <c r="N17">
-        <v>1.012701146323788</v>
+        <v>1.012701146323787</v>
       </c>
       <c r="O17">
         <v>1.03</v>
       </c>
       <c r="P17">
-        <v>1.028704746626986</v>
+        <v>1.028704746626985</v>
       </c>
       <c r="Q17">
         <v>1.02</v>
       </c>
       <c r="R17">
-        <v>1.02798750722522</v>
+        <v>1.027987507225219</v>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -1281,13 +1281,13 @@
         <v>1.05</v>
       </c>
       <c r="C18">
-        <v>0.9834017480067438</v>
+        <v>0.9834017480067445</v>
       </c>
       <c r="D18">
         <v>1.01012523344355</v>
       </c>
       <c r="E18">
-        <v>0.9913466192668643</v>
+        <v>0.9913466192668645</v>
       </c>
       <c r="F18">
         <v>1.009640145389163</v>
@@ -1311,13 +1311,13 @@
         <v>1.023294526548452</v>
       </c>
       <c r="N18">
-        <v>1.012542710423598</v>
+        <v>1.012542710423599</v>
       </c>
       <c r="O18">
         <v>1.03</v>
       </c>
       <c r="P18">
-        <v>1.027914880964075</v>
+        <v>1.027914880964076</v>
       </c>
       <c r="Q18">
         <v>1.02</v>
@@ -1340,16 +1340,16 @@
         <v>1.009065968647237</v>
       </c>
       <c r="E19">
-        <v>0.9894995744642792</v>
+        <v>0.9894995744642795</v>
       </c>
       <c r="F19">
-        <v>1.007676678029155</v>
+        <v>1.007676678029154</v>
       </c>
       <c r="G19">
         <v>1</v>
       </c>
       <c r="I19">
-        <v>1.04241271711888</v>
+        <v>1.042412717118881</v>
       </c>
       <c r="J19">
         <v>1.009564812533685</v>
@@ -1361,22 +1361,22 @@
         <v>1.003436522840021</v>
       </c>
       <c r="M19">
-        <v>1.021300365010519</v>
+        <v>1.021300365010518</v>
       </c>
       <c r="N19">
-        <v>1.010998510366186</v>
+        <v>1.010998510366185</v>
       </c>
       <c r="O19">
         <v>1.03</v>
       </c>
       <c r="P19">
-        <v>1.026007969484761</v>
+        <v>1.02600796948476</v>
       </c>
       <c r="Q19">
         <v>1.02</v>
       </c>
       <c r="R19">
-        <v>1.027172763870867</v>
+        <v>1.027172763870868</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -1387,13 +1387,13 @@
         <v>1.05</v>
       </c>
       <c r="C20">
-        <v>0.9755030342653198</v>
+        <v>0.9755030342653205</v>
       </c>
       <c r="D20">
-        <v>1.004498249179648</v>
+        <v>1.004498249179649</v>
       </c>
       <c r="E20">
-        <v>0.9829224150741076</v>
+        <v>0.9829224150741084</v>
       </c>
       <c r="F20">
         <v>1.001703062901288</v>
@@ -1402,22 +1402,22 @@
         <v>1</v>
       </c>
       <c r="I20">
-        <v>1.040254977949103</v>
+        <v>1.040254977949104</v>
       </c>
       <c r="J20">
         <v>1.004012063854953</v>
       </c>
       <c r="K20">
-        <v>1.018462460782616</v>
+        <v>1.018462460782617</v>
       </c>
       <c r="L20">
-        <v>0.9972723505243898</v>
+        <v>0.9972723505243904</v>
       </c>
       <c r="M20">
         <v>1.015716031959096</v>
       </c>
       <c r="N20">
-        <v>1.00543787614742</v>
+        <v>1.005437876147421</v>
       </c>
       <c r="O20">
         <v>1.03</v>
@@ -1429,7 +1429,7 @@
         <v>1.02</v>
       </c>
       <c r="R20">
-        <v>1.024204425267941</v>
+        <v>1.024204425267942</v>
       </c>
     </row>
     <row r="21" spans="1:18">
@@ -1440,16 +1440,16 @@
         <v>1.05</v>
       </c>
       <c r="C21">
-        <v>0.9660322925268648</v>
+        <v>0.9660322925268653</v>
       </c>
       <c r="D21">
-        <v>0.9978884357112571</v>
+        <v>0.9978884357112578</v>
       </c>
       <c r="E21">
-        <v>0.9746074984499101</v>
+        <v>0.9746074984499109</v>
       </c>
       <c r="F21">
-        <v>0.9956723945727697</v>
+        <v>0.9956723945727689</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -1458,19 +1458,19 @@
         <v>1.037400751528685</v>
       </c>
       <c r="J21">
-        <v>0.9970221897044722</v>
+        <v>0.9970221897044727</v>
       </c>
       <c r="K21">
-        <v>1.012909923056338</v>
+        <v>1.012909923056339</v>
       </c>
       <c r="L21">
-        <v>0.9900864551886286</v>
+        <v>0.9900864551886294</v>
       </c>
       <c r="M21">
-        <v>1.010736221228124</v>
+        <v>1.010736221228123</v>
       </c>
       <c r="N21">
-        <v>0.9984380755738962</v>
+        <v>0.9984380755738967</v>
       </c>
       <c r="O21">
         <v>1.03</v>
@@ -1482,7 +1482,7 @@
         <v>1.02</v>
       </c>
       <c r="R21">
-        <v>1.020281785252613</v>
+        <v>1.020281785252614</v>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -1493,16 +1493,16 @@
         <v>1.05</v>
       </c>
       <c r="C22">
-        <v>0.9599724758478494</v>
+        <v>0.9599724758478506</v>
       </c>
       <c r="D22">
-        <v>0.9936660442728837</v>
+        <v>0.9936660442728846</v>
       </c>
       <c r="E22">
-        <v>0.9693143804275052</v>
+        <v>0.9693143804275064</v>
       </c>
       <c r="F22">
-        <v>0.9919599863038138</v>
+        <v>0.9919599863038132</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -1511,31 +1511,31 @@
         <v>1.03556542043094</v>
       </c>
       <c r="J22">
-        <v>0.9925758973997004</v>
+        <v>0.9925758973997013</v>
       </c>
       <c r="K22">
-        <v>1.009364031069234</v>
+        <v>1.009364031069235</v>
       </c>
       <c r="L22">
-        <v>0.9855192599423414</v>
+        <v>0.9855192599423426</v>
       </c>
       <c r="M22">
         <v>1.00769241792275</v>
       </c>
       <c r="N22">
-        <v>0.9939854690240547</v>
+        <v>0.9939854690240557</v>
       </c>
       <c r="O22">
         <v>1.03</v>
       </c>
       <c r="P22">
-        <v>1.014659944167829</v>
+        <v>1.014659944167828</v>
       </c>
       <c r="Q22">
         <v>1.02</v>
       </c>
       <c r="R22">
-        <v>1.017760831068085</v>
+        <v>1.017760831068086</v>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -1552,10 +1552,10 @@
         <v>0.9958718579157801</v>
       </c>
       <c r="E23">
-        <v>0.9720614375993992</v>
+        <v>0.9720614375993994</v>
       </c>
       <c r="F23">
-        <v>0.993913067512776</v>
+        <v>0.9939130675127756</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -1564,25 +1564,25 @@
         <v>1.036522593768621</v>
       </c>
       <c r="J23">
-        <v>0.9948920919012861</v>
+        <v>0.9948920919012862</v>
       </c>
       <c r="K23">
         <v>1.011210820940264</v>
       </c>
       <c r="L23">
-        <v>0.9878812614800251</v>
+        <v>0.9878812614800254</v>
       </c>
       <c r="M23">
         <v>1.009290447419173</v>
       </c>
       <c r="N23">
-        <v>0.9963049527875042</v>
+        <v>0.9963049527875041</v>
       </c>
       <c r="O23">
         <v>1.03</v>
       </c>
       <c r="P23">
-        <v>1.015924723719003</v>
+        <v>1.015924723719002</v>
       </c>
       <c r="Q23">
         <v>1.02</v>
@@ -1599,16 +1599,16 @@
         <v>1.05</v>
       </c>
       <c r="C24">
-        <v>0.9752437610463732</v>
+        <v>0.9752437610463742</v>
       </c>
       <c r="D24">
         <v>1.00430233368467</v>
       </c>
       <c r="E24">
-        <v>0.9825771743111142</v>
+        <v>0.9825771743111151</v>
       </c>
       <c r="F24">
-        <v>1.001393753205032</v>
+        <v>1.001393753205033</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -1617,13 +1617,13 @@
         <v>1.040147545907646</v>
       </c>
       <c r="J24">
-        <v>1.003729251431278</v>
+        <v>1.003729251431279</v>
       </c>
       <c r="K24">
         <v>1.018254314441634</v>
       </c>
       <c r="L24">
-        <v>0.9969173222465462</v>
+        <v>0.9969173222465472</v>
       </c>
       <c r="M24">
         <v>1.015396437104479</v>
@@ -1652,16 +1652,16 @@
         <v>1.05</v>
       </c>
       <c r="C25">
-        <v>0.9883551633266554</v>
+        <v>0.9883551633266556</v>
       </c>
       <c r="D25">
         <v>1.013465881755529</v>
       </c>
       <c r="E25">
-        <v>0.9939805336729689</v>
+        <v>0.9939805336729691</v>
       </c>
       <c r="F25">
-        <v>1.009606546978454</v>
+        <v>1.009606546978452</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -1673,13 +1673,13 @@
         <v>1.013280879880571</v>
       </c>
       <c r="K25">
-        <v>1.025858692800031</v>
+        <v>1.025858692800032</v>
       </c>
       <c r="L25">
         <v>1.006673018389107</v>
       </c>
       <c r="M25">
-        <v>1.022057541857143</v>
+        <v>1.022057541857141</v>
       </c>
       <c r="N25">
         <v>1.014719854954943</v>
@@ -1688,7 +1688,7 @@
         <v>1.03</v>
       </c>
       <c r="P25">
-        <v>1.02602930693236</v>
+        <v>1.026029306932358</v>
       </c>
       <c r="Q25">
         <v>1.02</v>

</xml_diff>